<commit_message>
create 8 files, update 11 files and copy 2 files
</commit_message>
<xml_diff>
--- a/public/export/ProductsDatas.xlsx
+++ b/public/export/ProductsDatas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>Code</t>
   </si>
@@ -29,76 +29,151 @@
     <t>Famille</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Prix de vente HT</t>
   </si>
   <si>
     <t>Unité</t>
   </si>
   <si>
+    <t>Compte comptable</t>
+  </si>
+  <si>
     <t>Clavier Mécanique Gaming RGB</t>
   </si>
   <si>
     <t>Produit</t>
   </si>
   <si>
+    <t>Clavier mécanique avec rétroéclairage RGB, pour le gaming.</t>
+  </si>
+  <si>
     <t>Pièce</t>
   </si>
   <si>
     <t>Souris Gamer 7200 DPI</t>
   </si>
   <si>
+    <t>Souris gaming haute précision avec 7200 DPI.</t>
+  </si>
+  <si>
     <t>Écran 24" Full HD</t>
   </si>
   <si>
+    <t>Écran 24 pouces Full HD, parfait pour le multitâche.</t>
+  </si>
+  <si>
     <t>Disque SSD 500 Go</t>
   </si>
   <si>
+    <t>Disque SSD rapide avec 500 Go de stockage.</t>
+  </si>
+  <si>
     <t>Barrette RAM 8 Go DDR4</t>
   </si>
   <si>
+    <t>Barrette de RAM DDR4 de 8 Go pour améliorer les performances.</t>
+  </si>
+  <si>
     <t>Carte Mère ATX Z490</t>
   </si>
   <si>
+    <t>Carte mère ATX compatible Z490 pour des configurations gaming.</t>
+  </si>
+  <si>
     <t>Carte Graphique RTX 3060</t>
   </si>
   <si>
+    <t>Carte graphique puissante RTX 3060 pour le gaming.</t>
+  </si>
+  <si>
     <t>Boîtier PC Gaming</t>
   </si>
   <si>
+    <t>Boîtier PC Gaming avec gestion des câbles et ventilation optimisée.</t>
+  </si>
+  <si>
     <t>Alimentation 650W 80+ Bronze</t>
   </si>
   <si>
+    <t>Alimentation 650W certifiée 80+ Bronze pour une meilleure efficacité.</t>
+  </si>
+  <si>
     <t>Ventirad Processeur</t>
   </si>
   <si>
+    <t>Ventirad processeur silencieux pour un refroidissement efficace.</t>
+  </si>
+  <si>
     <t>Clavier Sans Fil Compact</t>
   </si>
   <si>
+    <t>Clavier compact sans fil, idéal pour les petits espaces.</t>
+  </si>
+  <si>
     <t>Hub USB 3.0 4 Ports</t>
   </si>
   <si>
+    <t>Hub USB 3.0 avec 4 ports pour connecter facilement vos périphériques.</t>
+  </si>
+  <si>
     <t>Câble HDMI 2.0 1,5m</t>
   </si>
   <si>
+    <t>Câble HDMI 2.0 de 1,5m pour une transmission vidéo optimale.</t>
+  </si>
+  <si>
     <t>Webcam Full HD 1080p</t>
   </si>
   <si>
+    <t>Webcam Full HD 1080p pour des visioconférences de qualité.</t>
+  </si>
+  <si>
     <t>Clé USB 64 Go</t>
   </si>
   <si>
+    <t>Clé USB de 64 Go pour le stockage de données portable.</t>
+  </si>
+  <si>
     <t>Support Écran Réglable</t>
   </si>
   <si>
+    <t>Support d’écran réglable pour un confort de vision optimal.</t>
+  </si>
+  <si>
     <t>Tapis de Souris XXL</t>
   </si>
   <si>
+    <t>Tapis de souris XXL pour une surface de jeu étendue.</t>
+  </si>
+  <si>
     <t>Chargeur USB Type-C Rapide</t>
   </si>
   <si>
+    <t>Chargeur rapide USB Type-C pour une recharge rapide et efficace.</t>
+  </si>
+  <si>
     <t>Casque Audio Gaming</t>
   </si>
   <si>
+    <t>Casque audio gaming avec un son immersif.</t>
+  </si>
+  <si>
     <t>Adaptateur USB-C vers HDMI</t>
+  </si>
+  <si>
+    <t>Adaptateur USB-C vers HDMI pour la connectivité de vos appareils.</t>
+  </si>
+  <si>
+    <t>azert</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>azerazeza</t>
   </si>
 </sst>
 </file>
@@ -439,15 +514,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="18.9954" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,345 +541,491 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1234567890123</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
         <v>58.33</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1234567890124</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>23.33</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>1234567890125</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
         <v>149.99</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>1234567890126</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
         <v>74.99</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>1234567890127</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6">
         <v>45.83</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>1234567890128</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
         <v>124.99</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>1234567890129</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8">
         <v>399.99</v>
       </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>1234567890130</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9">
         <v>83.33</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>1234567890131</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
         <v>66.66</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>1234567890132</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
         <v>29.16</v>
       </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>1234567890133</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12">
         <v>33.33</v>
       </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>1234567890134</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13">
         <v>16.66</v>
       </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>1234567890135</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14">
         <v>8.33</v>
       </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>1234567890136</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15">
         <v>33.33</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>1234567890137</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16">
         <v>16.66</v>
       </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>1234567890138</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17">
         <v>23.33</v>
       </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>1234567890139</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18">
         <v>20.83</v>
       </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>1234567890140</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19">
         <v>23.33</v>
       </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>1234567890141</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20">
         <v>54.16</v>
       </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>1234567890142</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21">
         <v>23.33</v>
       </c>
-      <c r="F21" t="s">
-        <v>8</v>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21">
+        <v>707000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23">
+        <v>8.33</v>
+      </c>
+      <c r="H23">
+        <v>706000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>